<commit_message>
Exercicio 1 Der criado
</commit_message>
<xml_diff>
--- a/Exercício 1- Agência de turismo/DER.xlsx
+++ b/Exercício 1- Agência de turismo/DER.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juninho\Desktop\Códigos Daniel\sql\Exercício 1- Agência de turismo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B763D6-B494-445A-9D7E-2925F9C9414F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1A1911-AF30-485D-92E9-29545B8C683B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{68DA10BA-544F-4ADD-9885-E61AAA45FE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
     <author>Juninho</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{727A7BD9-8849-4B55-9590-8345CBEF6015}">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{3AD20DA8-85BC-4A4A-82CD-833AD6A751A7}">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{29CE17EB-DB93-4488-9180-91C87C06338A}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{727A7BD9-8849-4B55-9590-8345CBEF6015}">
       <text>
         <r>
           <rPr>
@@ -80,12 +80,84 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
+          <t>IDENTITY, PRIMARY KEY</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{697E79FE-F08B-4992-AEAD-ED6CE4C2457D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>UNIQUE, NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{29CE17EB-DB93-4488-9180-91C87C06338A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">NOT NULL, CHECK(quartos IN('Simples', 'Mediano', 'Luxo', 'Superluxo')
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{08C422C9-FE55-4A3F-A249-7C8ED18BE5F2}">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{064E3F41-FF46-4580-9899-ED81ED91C2FF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{08C422C9-FE55-4A3F-A249-7C8ED18BE5F2}">
       <text>
         <r>
           <rPr>
@@ -109,7 +181,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{BAA9B558-D895-491A-B7FC-0E7D709370D0}">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{EB0EAD13-51D6-4231-8037-2C63AC72C889}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">NOT NULL
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{BAA9B558-D895-491A-B7FC-0E7D709370D0}">
       <text>
         <r>
           <rPr>
@@ -157,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{F8159A6D-72C0-4810-A908-CB4851098BA0}">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{28D73158-AE82-4EB2-ABDD-1EA666354D04}">
       <text>
         <r>
           <rPr>
@@ -177,11 +274,60 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-FOREIGN KEY REFERENCES hoteis(codigo)</t>
+NOT NULL, CHECK(tipoConstrucao IN('Comum', 'Barroca', 'Santuário', 'Templo', 'Catedral', 'Convento')</t>
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{1D6100FD-4684-4D7A-8741-126EE5788C0F}">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{F8159A6D-72C0-4810-A908-CB4851098BA0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>CONSTRAINTS</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+NOT NULL  FOREIGN KEY REFERENCES hoteis(codigo)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{6F16296D-C607-4009-BEB1-0AADF37C2869}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOT NULL FOREIGN KEY REFERENCES
+cidades(codigo)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{1D6100FD-4684-4D7A-8741-126EE5788C0F}">
       <text>
         <r>
           <rPr>
@@ -205,7 +351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{1B7C51BD-2755-417F-9EE3-695BB0DF363D}">
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{1B7C51BD-2755-417F-9EE3-695BB0DF363D}">
       <text>
         <r>
           <rPr>
@@ -229,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{A273ACDE-1179-472C-A64F-68B44884205C}">
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{08F919CE-3908-4CB2-9CBF-625EBDEDD6B9}">
       <text>
         <r>
           <rPr>
@@ -239,20 +385,21 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">CONSTRAINTS </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">UNIQUE, NOT NULL </t>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>IDENTITY, PRIMARY KEY</t>
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{C339642F-B9C1-4F17-AE62-CDB146653CB2}">
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{4DDE0411-44CC-413D-924E-C2D00D6FF992}">
       <text>
         <r>
           <rPr>
@@ -262,20 +409,21 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">CONSTRAINTS </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">UNIQUE, NOT NULL </t>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>IDENTITY, PRIMARY KEY</t>
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{EC7DD163-5996-47F3-B5DE-9C9B29ED8FA1}">
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{381EBF6F-F808-4279-9AF9-875083598D3E}">
       <text>
         <r>
           <rPr>
@@ -295,11 +443,152 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>UNIQUE, NOT NULL</t>
+          <t>IDENTITY, PRIMARY KEY</t>
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{755C158C-2D81-4206-B7AB-33A443A716E9}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{A273ACDE-1179-472C-A64F-68B44884205C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">UNIQUE, NOT NULL </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{C339642F-B9C1-4F17-AE62-CDB146653CB2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">UNIQUE, NOT NULL </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{E2832C86-E100-4F42-9117-170AC022DAF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>UNIQUE, NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{919BC41A-CDC4-4FAC-899C-90F293CDCDCD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>CONSTRAINTS</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+NOT NULL FOREIGN KEY REFERENCES museus(codigo)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{348C51FA-740F-44EC-AC96-4C9C0D04FEF3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">UNIQUE, NOT NULL </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{EC7DD163-5996-47F3-B5DE-9C9B29ED8FA1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>UNIQUE, NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{755C158C-2D81-4206-B7AB-33A443A716E9}">
       <text>
         <r>
           <rPr>
@@ -323,7 +612,80 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{7D97F083-4D9F-4A3D-B6A0-414D08A329CD}">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{FD93D4B1-9192-49E6-86EF-AF0BD05824D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{AB0B751E-FCA2-45D5-9945-07457C717D83}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOT NULL FOREIGN KEY REFERENCES fundadores(codigo)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{23DC88B6-BD21-4A1B-ADD0-618AF690E908}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">NOT NULL
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{7D97F083-4D9F-4A3D-B6A0-414D08A329CD}">
       <text>
         <r>
           <rPr>
@@ -347,7 +709,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{4474E1AD-7B59-4036-9AE6-BCDC16167BF4}">
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{4474E1AD-7B59-4036-9AE6-BCDC16167BF4}">
       <text>
         <r>
           <rPr>
@@ -371,7 +733,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{D6D0B070-B2FF-4664-BE83-FAF506E50208}">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{9A70434D-60BD-4826-AF34-6BB4BC74E553}">
       <text>
         <r>
           <rPr>
@@ -391,8 +753,586 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">NOT NULL
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{BF57B5C4-3A3C-4F2C-AE80-AA7BE0D3185A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+OBS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">SE HOUVER
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{D6D0B070-B2FF-4664-BE83-FAF506E50208}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOT NULL FOREIGN KEY REFERENCES
+cidades(codigo)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{ACD8E7F4-B04A-4A2B-8C60-31804084E979}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">NOT NULL
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J15" authorId="0" shapeId="0" xr:uid="{3E681AC7-941C-45B8-A92F-FC6597D30C29}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">NOT NULL
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{D80782CF-46F6-4E93-B63E-F8275866FF1E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>FOREIGN KEY REFERENCES
+restaurantes(codigo)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{D088FE41-9EF7-4D62-AA82-1C55A55AFA8A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOT NULL FOREIGN KEY REFERENCES
+cidades(codigo)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{E106B7C0-3C1B-4FEF-AF9B-F43D7F37F572}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">NOT NULL
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{69C5D600-A8C8-4AF0-B0D3-4A96CC6A5FBC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">IDENTITY, PRIMARY KEY
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{CF1DD306-68BA-47B9-8BD4-79009A24990F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>IDENTITY, PRIMARY KEY</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{873A8F6C-D8A4-4000-8BB9-87C586EEAF29}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">UNIQUE, NOT NULL </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{55E71141-922B-4A6F-BD3D-99D706D5DC8B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>UNIQUE, NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{BE261E41-17BB-4CBE-9C11-5E6244966FAD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>UNIQUE, NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E21" authorId="0" shapeId="0" xr:uid="{732AE742-570C-4BC2-A5C9-5819601F9186}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOT NULL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{0FE5489E-B444-4BF9-BF4D-925FF361BBA7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>CONSTRAINTS</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+NOT NULL, CHECK(categoria IN('Simples', 'Mediano', 'Luxo', 'Superluxo')</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{4E34C0A6-500E-4289-B02B-9294A5FB1372}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOT NULL</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+OBS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">IGUAL PARA TODOS OS DIAS DA SEMANA
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{95C6FEF5-20CE-4654-B3C6-7ED8DF68D7F5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">NOT NULL
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{EE8BB831-2A93-4319-8EC9-CB69A019BF7A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">NOT NULL
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">OBS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>APENAS UM DIA DA SEMANA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="0" shapeId="0" xr:uid="{FF17C296-BCDF-43B1-A392-56FB58D94DFE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">NOT NULL, CHECK(especialidade IN('Chinesa', 'Japonesa', 'Italiana', 'Fast Food', 'Brasileira')
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E24" authorId="0" shapeId="0" xr:uid="{D072E4CF-7ABD-4203-A02A-7B82F0564E09}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOT NULL FOREIGN KEY REFERENCES
+cidades(codigo)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C25" authorId="0" shapeId="0" xr:uid="{060F87D8-AA3C-44B7-BA08-A5D54B6B04EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOT NULL</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
           <t>FOREIGN KEY REFERENCES
 cidades(codigo)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E25" authorId="0" shapeId="0" xr:uid="{B07A2574-99A7-4593-A124-792F00CBCE8C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CONSTRAINTS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>FOREIGN KEY REFERENCES
+restaurantes(codigo)</t>
         </r>
       </text>
     </comment>
@@ -401,7 +1341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>hoteis</t>
   </si>
@@ -450,6 +1390,69 @@
   <si>
     <t>cidade TINYINT</t>
   </si>
+  <si>
+    <t>restaurantes</t>
+  </si>
+  <si>
+    <t>restaurante TINYINT</t>
+  </si>
+  <si>
+    <t>igrejas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">descricao VARCHAR(500) </t>
+  </si>
+  <si>
+    <t>dataCriacao DATETIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tipoConstrucao VARCHAR(20) </t>
+  </si>
+  <si>
+    <t>casasDeShow</t>
+  </si>
+  <si>
+    <t>horarioInicioShow TIME</t>
+  </si>
+  <si>
+    <t>diaFechamento DATETIME</t>
+  </si>
+  <si>
+    <t>precoMedio DECIMAL(5,2)</t>
+  </si>
+  <si>
+    <t>especialidade VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>museus</t>
+  </si>
+  <si>
+    <t>numeroSalas SMALLINT</t>
+  </si>
+  <si>
+    <t>fundador TINYINT</t>
+  </si>
+  <si>
+    <t>museu TINYINT</t>
+  </si>
+  <si>
+    <t>fundar</t>
+  </si>
+  <si>
+    <t>fundadores</t>
+  </si>
+  <si>
+    <t>dataNascimento DATETIME</t>
+  </si>
+  <si>
+    <t>dataMorte DATETIME</t>
+  </si>
+  <si>
+    <t>nacionalidade VARCHAR(30)</t>
+  </si>
+  <si>
+    <t>profissao VARCHAR(30)</t>
+  </si>
 </sst>
 </file>
 
@@ -493,7 +1496,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -542,8 +1545,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB9B9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -615,24 +1654,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color theme="1"/>
       </left>
@@ -643,11 +1664,127 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -665,15 +1802,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -684,16 +1812,90 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFB9B9"/>
+      <color rgb="FFFF8989"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -709,15 +1911,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>1007205</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -773,15 +1975,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>762001</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>762683</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>184483</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -825,15 +2027,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>1007205</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>1552074</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>24064</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -877,9 +2079,9 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>937260</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="258789" cy="264560"/>
@@ -935,9 +2137,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="256160" cy="264560"/>
@@ -993,15 +2195,15 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>1083405</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1057,16 +2259,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>1083405</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>100519</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>101816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1582366</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>101816</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1676400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1083,8 +2285,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6514682" y="2003898"/>
-          <a:ext cx="498961" cy="1297"/>
+          <a:off x="6516465" y="2014436"/>
+          <a:ext cx="592995" cy="1054"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1109,15 +2311,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>3717</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>104474</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>601692</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>104475</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1159,9 +2361,9 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>1006103</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>63588</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="256160" cy="264560"/>
@@ -1217,9 +2419,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>454048</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>64114</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="258789" cy="264560"/>
@@ -1237,6 +2439,2080 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5887896" y="1782555"/>
+          <a:ext cx="258789" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>n</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>999585</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Fluxograma: Decisão 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0044301-A999-4C09-A756-CD328585E05E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4389120" y="3154680"/>
+          <a:ext cx="489045" cy="327660"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>830580</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1319625</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Fluxograma: Decisão 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{884F3EF6-5BF9-4CD5-B624-C1976F99FB13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7848600" y="3154680"/>
+          <a:ext cx="489045" cy="327660"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>753980</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>753980</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>144378</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Conector reto 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDCE86EB-3ECD-4075-B36E-80BD8ECDE591}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4632560" y="2842260"/>
+          <a:ext cx="0" cy="327258"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>982580</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>108183</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>108184</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Conector reto 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EEED0CA-DA50-4CF0-AF3B-06F1DCCCD1C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4859255" y="3308583"/>
+          <a:ext cx="560470" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>108183</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>842962</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>108183</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Conector reto 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0AB1D4B-A2F4-47ED-9017-FEC828D5BA30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7034213" y="3308583"/>
+          <a:ext cx="823912" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1073067</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1073067</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>131995</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Conector reto 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A668949A-5D5B-4F82-8DB9-D4D6E174DA3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8088230" y="2466975"/>
+          <a:ext cx="0" cy="684445"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>930691</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>98009</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="256160" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="CaixaDeTexto 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DCD5303-E00D-485E-A7FE-561545888FEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4809271" y="3306029"/>
+          <a:ext cx="256160" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>500556</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>106155</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="256160" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="CaixaDeTexto 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E175532A-5A33-4537-A1F7-D4D754F930EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4379136" y="2940795"/>
+          <a:ext cx="256160" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1044991</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>98009</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="256160" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="CaixaDeTexto 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3172A0E-841F-4BC7-BB64-8FAC19CA9646}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8063011" y="2932649"/>
+          <a:ext cx="256160" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>645336</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>90915</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="258789" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="CaixaDeTexto 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5596AFBD-22AA-4B95-B0E0-EE8449F27CE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7663356" y="3321795"/>
+          <a:ext cx="258789" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>n</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1205325</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Fluxograma: Decisão 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E958D4DE-185E-43F7-97B8-0DE45F9DDA24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9784080" y="1805940"/>
+          <a:ext cx="489045" cy="350520"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>953183</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>188595</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>955910</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Conector reto 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F76708FB-4525-4D75-B05E-DDAC664C621D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10020983" y="1323975"/>
+          <a:ext cx="2727" cy="489585"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>70083</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>725805</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>70083</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Conector reto 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C3C789C-307D-421D-A60D-63671C5C26C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9075420" y="1975083"/>
+          <a:ext cx="718185" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>526831</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>37049</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="256160" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="CaixaDeTexto 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDE1B916-32B2-448F-A75D-D003C01D0482}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9594631" y="1949669"/>
+          <a:ext cx="256160" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>927276</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>75675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="258789" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="CaixaDeTexto 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F292D81C-941F-4883-9511-90183F6CA866}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9995076" y="1599675"/>
+          <a:ext cx="258789" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>n</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1327245</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Fluxograma: Decisão 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E9BC6B2-3BE0-4993-BB4C-F847256990BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7962900" y="3802380"/>
+          <a:ext cx="489045" cy="350520"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>16193</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>176763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>840105</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>176763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Conector reto 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6DE5B1D-D314-4091-ADB6-1EF84FB95411}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7140893" y="3971523"/>
+          <a:ext cx="823912" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1327245</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2036445</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1503</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Conector reto 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97017CFC-F852-4588-AA8E-30D720361C5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="39" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8451945" y="3977640"/>
+          <a:ext cx="709200" cy="1503"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>656371</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>128489</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="256160" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="CaixaDeTexto 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B52A4EE3-5F84-4EDA-B675-3F8C607CCC84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7781071" y="3740369"/>
+          <a:ext cx="256160" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1250731</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>128489</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="256160" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="CaixaDeTexto 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAAF742C-2B3A-42E1-AF14-0EACD4AD55AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8375431" y="3740369"/>
+          <a:ext cx="256160" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1205325</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="Fluxograma: Decisão 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE220EAC-64C1-4B11-B021-FACC5D13962F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9890760" y="2225040"/>
+          <a:ext cx="489045" cy="350520"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>115803</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>725805</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>115803</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="Conector reto 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4253FEAF-8C82-4D1C-A1A9-799EBF0AF29E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9182100" y="2394183"/>
+          <a:ext cx="718185" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1205325</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>115803</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1906</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Conector reto 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{001506E4-F4CC-4F00-9679-50213E5660E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="46" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10379805" y="2394183"/>
+          <a:ext cx="633001" cy="6117"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1133016</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>60435</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="258789" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="CaixaDeTexto 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7667C03D-8E44-411C-9B49-5430B5F142C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10307496" y="2155935"/>
+          <a:ext cx="258789" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>n</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>526831</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>75149</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="256160" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="CaixaDeTexto 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3573B3D2-0A60-498E-9FD9-60BC27C39F26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9701311" y="2170649"/>
+          <a:ext cx="256160" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>892905</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Fluxograma: Decisão 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27F299B7-5E81-4999-AAAB-B73E09FE392B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9700260" y="2011680"/>
+          <a:ext cx="489045" cy="350520"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>868681</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85323</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="Conector reto 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95105637-2E27-40CF-9974-E26382106F3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10165081" y="2188443"/>
+          <a:ext cx="365759" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>77703</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>426721</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>77703</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Conector reto 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{825124BC-1B37-4FA8-99F8-D60242BBC43F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9319260" y="2180823"/>
+          <a:ext cx="403861" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>988236</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>45195</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="258789" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="CaixaDeTexto 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E60236F3-DFBA-49DE-AA90-237082365F92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10284636" y="1957815"/>
+          <a:ext cx="258789" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>n</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>206791</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>52289</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="256160" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="CaixaDeTexto 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5546EE7D-7476-4136-8A03-7AA818A70D48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9503191" y="1964909"/>
+          <a:ext cx="256160" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>206791</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>52289</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="CaixaDeTexto 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1735454-EF30-49B6-B7E6-F598F34677F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11850151" y="2155409"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>892905</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="Fluxograma: Decisão 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A99730D-9D9E-4AB9-8791-D816A873CC7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9700260" y="2011680"/>
+          <a:ext cx="489045" cy="350520"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>868682</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1303020</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85323</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="Conector reto 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98B4A9AA-739D-42CC-B433-FDA965F0B94C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12512042" y="2188443"/>
+          <a:ext cx="434338" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>77703</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>426721</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>77703</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Conector reto 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60480859-2AA8-447C-9E24-5E08A78154B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9319260" y="2180823"/>
+          <a:ext cx="403861" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>988236</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>45195</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="CaixaDeTexto 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68274367-D69A-4B31-8ADD-F61CB233F74A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12631596" y="1957815"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>816391</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>44669</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="256160" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="CaixaDeTexto 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFAB25D0-E544-49A9-97E9-9B0D28F3FA67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12459751" y="1957289"/>
+          <a:ext cx="256160" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>226236</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>29955</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="258789" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="83" name="CaixaDeTexto 82">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDE162E9-60C5-45E5-97B5-FB379E30175D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11869596" y="1942575"/>
           <a:ext cx="258789" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1579,25 +4855,25 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
+    <col min="10" max="10" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1622,12 +4898,12 @@
     <row r="2" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1649,15 +4925,17 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="10" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1679,15 +4957,17 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="C4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1711,13 +4991,15 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2"/>
+      <c r="E5" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1741,13 +5023,15 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1769,15 +5053,17 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1799,12 +5085,16 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="28" t="s">
+        <v>15</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1829,19 +5119,15 @@
     </row>
     <row r="9" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="45"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="45"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -1859,23 +5145,27 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
+      <c r="B10" s="16" t="s">
+        <v>0</v>
+      </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="D10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="31"/>
+      <c r="F10" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="40"/>
+      <c r="H10" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="40"/>
+      <c r="J10" s="46" t="s">
+        <v>32</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1893,21 +5183,29 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="B11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="31"/>
+      <c r="F11" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="49"/>
+      <c r="H11" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="49"/>
+      <c r="J11" s="50" t="s">
+        <v>6</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1927,21 +5225,25 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="10" t="s">
+        <v>1</v>
+      </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="48" t="s">
+        <v>30</v>
+      </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="42" t="s">
+        <v>1</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1961,19 +5263,27 @@
     </row>
     <row r="13" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="6" t="s">
-        <v>13</v>
+      <c r="B13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="47" t="s">
+        <v>19</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="H13" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="43" t="s">
+        <v>33</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1991,19 +5301,25 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+    <row r="14" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="18"/>
+      <c r="B14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="48" t="s">
+        <v>20</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="43" t="s">
+        <v>34</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -2021,17 +5337,23 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="1"/>
+      <c r="B15" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="48" t="s">
+        <v>28</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="43" t="s">
+        <v>35</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -2049,17 +5371,23 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="44" t="s">
+        <v>15</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="44" t="s">
+        <v>36</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -2077,13 +5405,13 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -2105,12 +5433,16 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="32" t="s">
+        <v>22</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -2133,12 +5465,16 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="C19" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="35" t="s">
+        <v>6</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2164,9 +5500,13 @@
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="C20" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="31"/>
+      <c r="E20" s="35" t="s">
+        <v>2</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -2192,9 +5532,13 @@
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="29" t="s">
+        <v>19</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -2219,10 +5563,14 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="33" t="s">
+        <v>23</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -2247,10 +5595,14 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="34" t="s">
+        <v>24</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2275,10 +5627,14 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="36" t="s">
+        <v>26</v>
+      </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="39" t="s">
+        <v>15</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -2301,12 +5657,16 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="40"/>
+      <c r="E25" s="30" t="s">
+        <v>17</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -2329,7 +5689,7 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>

</xml_diff>

<commit_message>
Exercicio 1- Tabelas criadas
</commit_message>
<xml_diff>
--- a/Exercício 1- Agência de turismo/DER.xlsx
+++ b/Exercício 1- Agência de turismo/DER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juninho\Desktop\Códigos Daniel\sql\Exercício 1- Agência de turismo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1A1911-AF30-485D-92E9-29545B8C683B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48C0886-7FC2-45D4-824A-EE0D1AD93917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{68DA10BA-544F-4ADD-9885-E61AAA45FE6E}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9072" xr2:uid="{68DA10BA-544F-4ADD-9885-E61AAA45FE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">NOT NULL, CHECK(quartos IN('Simples', 'Mediano', 'Luxo', 'Superluxo')
+          <t xml:space="preserve">NOT NULL, CHECK(tipo IN('Simples', 'Mediano', 'Luxo', 'Superluxo')
 </t>
         </r>
       </text>
@@ -1169,6 +1169,29 @@
           </rPr>
           <t xml:space="preserve">NOT NULL
 </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>OBS</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+TIPO 1: RS15,00
+TIPO 2: RS30,00
+TIPO 3: RS90,00
+TIPO 4: RS360,00</t>
         </r>
       </text>
     </comment>
@@ -1377,9 +1400,6 @@
   </si>
   <si>
     <t>cidades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estadoPertencente VARCHAR(40) </t>
   </si>
   <si>
     <t>populacao INT</t>
@@ -1452,6 +1472,9 @@
   </si>
   <si>
     <t>profissao VARCHAR(30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estadoPertencente VARCHAR(4) </t>
   </si>
 </sst>
 </file>
@@ -4549,6 +4572,286 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1394460</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1883505</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Fluxograma: Decisão 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7F692E2-37C0-4727-A7B6-65C9D710BA9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5250180" y="3368040"/>
+          <a:ext cx="489045" cy="365760"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1853026</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Conector reto 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D9173D6-DAE2-4178-A418-F2463BD55C8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5708746" y="3543300"/>
+          <a:ext cx="196754" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1641710</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1641710</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>128185</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Conector reto 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB8F2D11-47BB-4093-B74C-C8DBF95F26BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5497430" y="2680335"/>
+          <a:ext cx="0" cy="693970"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1834056</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>83295</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="258789" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="CaixaDeTexto 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{518C3AAC-9AFD-4CEF-B4C8-FE0D4686770D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5689776" y="3527535"/>
+          <a:ext cx="258789" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>n</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1395511</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>98009</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="256160" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="CaixaDeTexto 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B42BA96-F0B3-4174-A011-7A334FAC4E87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5251231" y="3146009"/>
+          <a:ext cx="256160" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4854,8 +5157,8 @@
   </sheetPr>
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4901,7 +5204,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -4997,7 +5300,7 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -5029,7 +5332,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -5061,7 +5364,7 @@
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -5093,7 +5396,7 @@
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -5156,15 +5459,15 @@
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="40"/>
       <c r="H10" s="46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" s="40"/>
       <c r="J10" s="46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -5189,7 +5492,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>6</v>
@@ -5238,7 +5541,7 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="42" t="s">
@@ -5267,22 +5570,22 @@
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I13" s="18"/>
       <c r="J13" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -5308,17 +5611,17 @@
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="18"/>
       <c r="J14" s="43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -5340,19 +5643,19 @@
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="18"/>
       <c r="F15" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="18"/>
       <c r="J15" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -5374,19 +5677,19 @@
     <row r="16" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="18"/>
       <c r="F16" s="44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="18"/>
       <c r="J16" s="44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -5437,11 +5740,11 @@
       <c r="A18" s="1"/>
       <c r="B18" s="18"/>
       <c r="C18" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -5537,7 +5840,7 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -5569,7 +5872,7 @@
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -5597,11 +5900,11 @@
       <c r="A23" s="1"/>
       <c r="B23" s="18"/>
       <c r="C23" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -5629,11 +5932,11 @@
       <c r="A24" s="1"/>
       <c r="B24" s="18"/>
       <c r="C24" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -5661,11 +5964,11 @@
       <c r="A25" s="1"/>
       <c r="B25" s="18"/>
       <c r="C25" s="38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" s="40"/>
       <c r="E25" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>

</xml_diff>